<commit_message>
SET NOCOUNT ON after OFF for some tests
</commit_message>
<xml_diff>
--- a/test/restest251.xlsx
+++ b/test/restest251.xlsx
@@ -440,13 +440,13 @@
     </row>
     <row r="4">
       <c r="B4">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="D4">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Added promise() for compiled statement
</commit_message>
<xml_diff>
--- a/test/restest251.xlsx
+++ b/test/restest251.xlsx
@@ -440,13 +440,13 @@
     </row>
     <row r="4">
       <c r="B4">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C4">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="D4">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
jsHint'ing the code. All tests OK
</commit_message>
<xml_diff>
--- a/test/restest251.xlsx
+++ b/test/restest251.xlsx
@@ -440,13 +440,13 @@
     </row>
     <row r="4">
       <c r="B4">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C4">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="D4">
-        <v>46</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Partial PIVOT (not working commit - to be fixed)
</commit_message>
<xml_diff>
--- a/test/restest251.xlsx
+++ b/test/restest251.xlsx
@@ -440,13 +440,13 @@
     </row>
     <row r="4">
       <c r="B4">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="D4">
-        <v>54</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Multiple tables for DROP TABLE
</commit_message>
<xml_diff>
--- a/test/restest251.xlsx
+++ b/test/restest251.xlsx
@@ -443,10 +443,10 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D4">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
PIVOT tests moved to skipped
</commit_message>
<xml_diff>
--- a/test/restest251.xlsx
+++ b/test/restest251.xlsx
@@ -440,13 +440,13 @@
     </row>
     <row r="4">
       <c r="B4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D4">
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
toJavaScript renamed to toJS. gulp+test ok
</commit_message>
<xml_diff>
--- a/test/restest251.xlsx
+++ b/test/restest251.xlsx
@@ -440,13 +440,13 @@
     </row>
     <row r="4">
       <c r="B4">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C4">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="D4">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5">

</xml_diff>